<commit_message>
Modelo conceitual feito e backlog sub atividades com datas
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog sprint 3.xlsx
+++ b/Documentação/Backlog/Backlog sprint 3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\BandTec\aulas ead 2º sem\Mind6\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4BFAF6-110D-40F4-A817-57EDA4DFECB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6ED1B6-EFC9-45E0-B442-5542D4BDB373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="88">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -270,6 +270,30 @@
   </si>
   <si>
     <t>Notas</t>
+  </si>
+  <si>
+    <t>27/11/2020</t>
+  </si>
+  <si>
+    <t>11/11/2020</t>
+  </si>
+  <si>
+    <t>13/11/2020</t>
+  </si>
+  <si>
+    <t>02/11/2020</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Pronto</t>
+  </si>
+  <si>
+    <t>Criar script para BD MYSQL</t>
+  </si>
+  <si>
+    <t>Vicari/Cesar/Yudi/Castione/Felipe</t>
   </si>
 </sst>
 </file>
@@ -309,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +376,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -857,7 +887,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -914,55 +944,19 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -974,64 +968,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1060,6 +1006,111 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1376,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F51"/>
+  <dimension ref="B1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22:F23"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,10 +1486,14 @@
       <c r="C4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9" t="s">
-        <v>9</v>
+      <c r="D4" s="69">
+        <v>44146</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1448,10 +1503,14 @@
       <c r="C5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="9" t="s">
-        <v>9</v>
+      <c r="D5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1461,8 +1520,12 @@
       <c r="C6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="F6" s="9" t="s">
         <v>9</v>
       </c>
@@ -1474,8 +1537,12 @@
       <c r="C7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="F7" s="9" t="s">
         <v>9</v>
       </c>
@@ -1487,8 +1554,12 @@
       <c r="C8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="F8" s="9" t="s">
         <v>9</v>
       </c>
@@ -1497,11 +1568,15 @@
       <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="F9" s="9" t="s">
         <v>9</v>
       </c>
@@ -1513,8 +1588,12 @@
       <c r="C10" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="F10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1526,8 +1605,12 @@
       <c r="C11" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="F11" s="9" t="s">
         <v>9</v>
       </c>
@@ -1539,8 +1622,12 @@
       <c r="C12" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="10"/>
+      <c r="D12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="F12" s="9" t="s">
         <v>9</v>
       </c>
@@ -1552,8 +1639,12 @@
       <c r="C13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="F13" s="9" t="s">
         <v>9</v>
       </c>
@@ -1565,52 +1656,52 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="66" t="s">
+      <c r="F16" s="38" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="30"/>
+      <c r="E17" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="54"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="35"/>
+      <c r="E18" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="59"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="13" t="s">
         <v>27</v>
       </c>
@@ -1620,96 +1711,96 @@
       <c r="E19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="35"/>
-    </row>
-    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="36"/>
-      <c r="C20" s="27" t="s">
+      <c r="F19" s="59"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="72"/>
+      <c r="C20" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="74"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="58"/>
+      <c r="C21" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D21" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="31"/>
-    </row>
-    <row r="21" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="60" t="s">
+      <c r="E21" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="55"/>
+    </row>
+    <row r="22" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C22" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D22" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="62"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
+      <c r="E22" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="34"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C23" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D23" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="25"/>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="26"/>
-      <c r="C23" s="27" t="s">
+      <c r="E23" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="43"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="42"/>
+      <c r="C24" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D24" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="28"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="59" t="s">
+      <c r="E24" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="44"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C25" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D25" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="52"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="16" t="s">
+      <c r="E25" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="50"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="52"/>
+      <c r="C26" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="52"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="C26" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>64</v>
@@ -1717,187 +1808,187 @@
       <c r="E26" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="52"/>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="58"/>
-      <c r="C27" s="22" t="s">
+      <c r="F26" s="50"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="52"/>
+      <c r="C27" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="50"/>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="53"/>
+      <c r="C28" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D28" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="52"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="s">
+      <c r="E28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="50"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C29" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D29" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="30"/>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="26"/>
-      <c r="C29" s="27" t="s">
+      <c r="E29" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="54"/>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="42"/>
+      <c r="C30" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D30" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="31"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="32" t="s">
+      <c r="E30" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="55"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C31" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D31" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="51"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="32"/>
-      <c r="C31" s="29" t="s">
+      <c r="E31" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="49"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="45"/>
+      <c r="C32" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D32" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="51"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="32"/>
-      <c r="C32" s="29" t="s">
+      <c r="E32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="49"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="45"/>
+      <c r="C33" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D33" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="49"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="45"/>
+      <c r="C34" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="51"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="32"/>
-      <c r="C33" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="29" t="s">
+      <c r="E34" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="49"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="45"/>
+      <c r="C35" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="51"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="32"/>
-      <c r="C34" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="29" t="s">
+      <c r="E35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="49"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="45"/>
+      <c r="C36" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="49"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="45"/>
+      <c r="C37" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="51"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="32"/>
-      <c r="C35" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="51"/>
-    </row>
-    <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="32"/>
-      <c r="C36" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="51"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="33" t="s">
+      <c r="E37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="49"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C38" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D38" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="30"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="34"/>
-      <c r="C38" s="13" t="s">
+      <c r="E38" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="54"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="57"/>
+      <c r="C39" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D39" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="35"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="34"/>
-      <c r="C39" s="13" t="s">
+      <c r="E39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="59"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="57"/>
+      <c r="C40" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="35"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="34"/>
-      <c r="C40" s="17" t="s">
-        <v>49</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>72</v>
@@ -1905,177 +1996,190 @@
       <c r="E40" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="35"/>
+      <c r="F40" s="59"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="34"/>
+      <c r="B41" s="57"/>
       <c r="C41" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="59"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="57"/>
+      <c r="C42" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D42" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="35"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="34"/>
-      <c r="C42" s="17" t="s">
+      <c r="E42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="59"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="57"/>
+      <c r="C43" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D43" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="35"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="34"/>
-      <c r="C43" s="17" t="s">
+      <c r="E43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="59"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="57"/>
+      <c r="C44" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D44" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="35"/>
-    </row>
-    <row r="44" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="36"/>
-      <c r="C44" s="37" t="s">
+      <c r="E44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="59"/>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="58"/>
+      <c r="C45" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="D45" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E44" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="31"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="32" t="s">
+      <c r="E45" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="55"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C46" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D46" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="57"/>
-    </row>
-    <row r="46" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="32"/>
-      <c r="C46" s="22" t="s">
+      <c r="E46" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="63"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="45"/>
+      <c r="C47" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D47" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="55"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="42" t="s">
+      <c r="E47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="64"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="43" t="s">
+      <c r="C48" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="43" t="s">
+      <c r="D48" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="44"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="45"/>
-      <c r="C48" s="46" t="s">
+      <c r="E48" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="46"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="61"/>
+      <c r="C49" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="46" t="s">
+      <c r="D49" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="47"/>
-    </row>
-    <row r="49" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="48"/>
-      <c r="C49" s="49" t="s">
+      <c r="E49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="47"/>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="62"/>
+      <c r="C50" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D49" s="49" t="s">
+      <c r="D50" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E49" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="50"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="40" t="s">
+      <c r="E50" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="48"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="38" t="s">
+      <c r="C51" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="67" t="s">
+      <c r="D51" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="E50" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="53"/>
-    </row>
-    <row r="51" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="41"/>
-      <c r="C51" s="39" t="s">
+      <c r="E51" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="67"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="66"/>
+      <c r="C52" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D51" s="68" t="s">
+      <c r="D52" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E51" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="54"/>
+      <c r="E52" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="F30:F36"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="B37:B44"/>
-    <mergeCell ref="F37:F44"/>
-    <mergeCell ref="B30:B36"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F31:F37"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="F38:F45"/>
+    <mergeCell ref="B31:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizando backlog, colocando select script sql, ajustando css na visao global
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog sprint 3.xlsx
+++ b/Documentação/Backlog/Backlog sprint 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\BandTec\aulas ead 2º sem\Mind6\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6ED1B6-EFC9-45E0-B442-5542D4BDB373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65096BF0-9D6B-4573-836B-939A4BA9AA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="88">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Diagrama de solução</t>
   </si>
   <si>
-    <t>Todos</t>
-  </si>
-  <si>
     <t>A fazer</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>Vicari</t>
   </si>
   <si>
-    <t>Vicari/Cesar/Castione</t>
-  </si>
-  <si>
     <t>Vicari/Cesar/Yudi/Castione</t>
   </si>
   <si>
@@ -293,7 +287,13 @@
     <t>Criar script para BD MYSQL</t>
   </si>
   <si>
-    <t>Vicari/Cesar/Yudi/Castione/Felipe</t>
+    <t>Trocar icone Telegram para Slack</t>
+  </si>
+  <si>
+    <t>Gráficos fundamentais sobre máquina</t>
+  </si>
+  <si>
+    <t>Felipe/Cesar/Cardoso</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -879,6 +879,21 @@
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -887,7 +902,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -980,15 +995,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,6 +1013,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1046,70 +1112,43 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="38" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1427,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F52"/>
+  <dimension ref="B1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,16 +1503,16 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="14">
         <v>44144</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>5</v>
@@ -1484,13 +1523,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="69">
+        <v>61</v>
+      </c>
+      <c r="D4" s="38">
         <v>44146</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>5</v>
@@ -1501,13 +1540,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>5</v>
@@ -1515,138 +1554,138 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>80</v>
-      </c>
       <c r="F12" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1656,531 +1695,559 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="56" t="s">
+      <c r="F16" s="35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="45"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="42"/>
+      <c r="C18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="46"/>
+    </row>
+    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="42"/>
+      <c r="C19" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="46"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="43"/>
+      <c r="C20" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="47"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="43"/>
+      <c r="C21" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="47"/>
+    </row>
+    <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="C22" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E22" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="54"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="57"/>
-      <c r="C18" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="13" t="s">
+      <c r="F22" s="77"/>
+    </row>
+    <row r="23" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="73"/>
+      <c r="C23" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="71" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="59"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="57"/>
-      <c r="C19" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="13" t="s">
+      <c r="E23" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="80"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="59"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="72"/>
-      <c r="C20" s="73" t="s">
+      <c r="E24" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="60"/>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="59"/>
+      <c r="C25" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="61"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="67"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="69"/>
+      <c r="C27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="67"/>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="69"/>
+      <c r="C28" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="67"/>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="70"/>
+      <c r="C29" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="67"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="45"/>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="59"/>
+      <c r="C31" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="48"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="66"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="62"/>
+      <c r="C33" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="D20" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="75" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="74"/>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="58"/>
-      <c r="C21" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="55"/>
-    </row>
-    <row r="22" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="34"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="43"/>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="42"/>
-      <c r="C24" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="44"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="50"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="52"/>
-      <c r="C26" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="50"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="52"/>
-      <c r="C27" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="50"/>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="53"/>
-      <c r="C28" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="50"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="54"/>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="42"/>
-      <c r="C30" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="55"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="49"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="45"/>
-      <c r="C32" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="49"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="45"/>
-      <c r="C33" s="24" t="s">
-        <v>42</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="49"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="45"/>
+      <c r="E33" s="83" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="66"/>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="62"/>
       <c r="C34" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="66"/>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="62"/>
+      <c r="C35" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="66"/>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="62"/>
+      <c r="C36" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="66"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="62"/>
+      <c r="C37" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="49"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="45"/>
-      <c r="C35" s="24" t="s">
+      <c r="D37" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="66"/>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="62"/>
+      <c r="C38" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="49"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="45"/>
-      <c r="C36" s="24" t="s">
+      <c r="D38" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="66"/>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="62"/>
+      <c r="C39" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="66"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D40" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="45"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="42"/>
+      <c r="C41" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="49"/>
-    </row>
-    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="45"/>
-      <c r="C37" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="49"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="54"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="57"/>
-      <c r="C39" s="13" t="s">
+      <c r="E41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="46"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="42"/>
+      <c r="C42" s="13" t="s">
         <v>47</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="59"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="57"/>
-      <c r="C40" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="59"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="57"/>
-      <c r="C41" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="59"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="57"/>
-      <c r="C42" s="17" t="s">
-        <v>50</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>70</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="59"/>
+        <v>8</v>
+      </c>
+      <c r="F42" s="46"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="57"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="46"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="42"/>
+      <c r="C44" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="46"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="42"/>
+      <c r="C45" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="46"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="42"/>
+      <c r="C46" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D46" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="46"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="44"/>
+      <c r="C47" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="59"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="57"/>
-      <c r="C44" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="13" t="s">
+      <c r="E47" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="48"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="59"/>
-    </row>
-    <row r="45" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="58"/>
-      <c r="C45" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="55"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" s="24" t="s">
+      <c r="E48" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="52"/>
+    </row>
+    <row r="49" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="62"/>
+      <c r="C49" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="63"/>
-    </row>
-    <row r="47" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="45"/>
-      <c r="C47" s="21" t="s">
+      <c r="D49" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="53"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D47" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="64"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="28" t="s">
+      <c r="D50" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="63"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="50"/>
+      <c r="C51" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="46"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="61"/>
-      <c r="C49" s="29" t="s">
+      <c r="D51" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="64"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="51"/>
+      <c r="C52" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="47"/>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="62"/>
-      <c r="C50" s="30" t="s">
+      <c r="D52" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="65"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E50" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="48"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="26" t="s">
+      <c r="D53" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="56"/>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="55"/>
+      <c r="C54" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="67"/>
-    </row>
-    <row r="52" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="66"/>
-      <c r="C52" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D52" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="E52" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="68"/>
+      <c r="D54" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="F40:F47"/>
+    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="F17:F21"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F31:F37"/>
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="F38:F45"/>
-    <mergeCell ref="B31:B37"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F32:F39"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="B40:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>